<commit_message>
update data and feature model
</commit_message>
<xml_diff>
--- a/Lehrplan21_Data/Lehrplan21asExcel.xlsx
+++ b/Lehrplan21_Data/Lehrplan21asExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kl/Desktop/bachelor/GitDez/BachelorThesisFeatureModel/Lehrplan21_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22262490-35F7-7E4B-98D4-CA995E2ABA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51AAF72-A990-BA48-B61F-975E7D029116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="29260" windowHeight="19020" xr2:uid="{9EF3264B-4CB2-F749-8DBA-EF109676CAB2}"/>
+    <workbookView xWindow="30200" yWindow="1060" windowWidth="45720" windowHeight="36820" xr2:uid="{9EF3264B-4CB2-F749-8DBA-EF109676CAB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Lehrplan 21 ohne MA.2" sheetId="1" r:id="rId1"/>
@@ -1255,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1270,6 +1270,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1757,13 +1760,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="105" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B245" sqref="B245:D245"/>
+    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J183" sqref="J183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="129.33203125" customWidth="1"/>
+    <col min="2" max="2" width="155.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
@@ -2727,13 +2730,13 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="12" t="s">
         <v>178</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="2">
@@ -3154,10 +3157,10 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" t="s">
         <v>41</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -3384,7 +3387,9 @@
         <v>3</v>
       </c>
       <c r="F72" s="2"/>
-      <c r="G72" s="8"/>
+      <c r="G72" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -3403,7 +3408,9 @@
         <v>3</v>
       </c>
       <c r="F73" s="2"/>
-      <c r="G73" s="8"/>
+      <c r="G73" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A74">
@@ -3423,6 +3430,9 @@
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="8"/>
+      <c r="J74" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -3442,6 +3452,9 @@
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="8"/>
+      <c r="J75" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -3463,6 +3476,9 @@
         <v>1</v>
       </c>
       <c r="G76" s="8"/>
+      <c r="H76" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -3484,6 +3500,9 @@
         <v>1</v>
       </c>
       <c r="G77" s="8"/>
+      <c r="J77" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -3503,6 +3522,9 @@
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="8"/>
+      <c r="J78" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -3522,6 +3544,9 @@
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="8"/>
+      <c r="J79" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -3541,8 +3566,11 @@
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="8"/>
-    </row>
-    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J80" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3560,8 +3588,11 @@
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="8"/>
-    </row>
-    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J81" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3579,8 +3610,11 @@
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="8"/>
-    </row>
-    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J82" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3597,9 +3631,11 @@
         <v>2</v>
       </c>
       <c r="F83" s="2"/>
-      <c r="G83" s="8"/>
-    </row>
-    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G83" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3619,8 +3655,11 @@
         <v>1</v>
       </c>
       <c r="G84" s="8"/>
-    </row>
-    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J84" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3640,8 +3679,11 @@
         <v>1</v>
       </c>
       <c r="G85" s="8"/>
-    </row>
-    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H85" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3659,8 +3701,11 @@
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="8"/>
-    </row>
-    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H86" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3677,9 +3722,11 @@
         <v>2.5</v>
       </c>
       <c r="F87" s="2"/>
-      <c r="G87" s="8"/>
-    </row>
-    <row r="88" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G87" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3697,8 +3744,11 @@
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="8"/>
-    </row>
-    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J88" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3716,8 +3766,11 @@
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="8"/>
-    </row>
-    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J89" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3735,8 +3788,11 @@
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="8"/>
-    </row>
-    <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J90" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3754,8 +3810,11 @@
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="8"/>
-    </row>
-    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H91" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3773,8 +3832,11 @@
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="8"/>
-    </row>
-    <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H92" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3791,9 +3853,11 @@
         <v>3</v>
       </c>
       <c r="F93" s="2"/>
-      <c r="G93" s="8"/>
-    </row>
-    <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G93" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3811,8 +3875,11 @@
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="8"/>
-    </row>
-    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J94" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3830,8 +3897,11 @@
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="8"/>
-    </row>
-    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J95" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3849,8 +3919,11 @@
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="8"/>
-    </row>
-    <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J96" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3868,8 +3941,11 @@
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="8"/>
-    </row>
-    <row r="98" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J97" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3889,8 +3965,11 @@
         <v>1</v>
       </c>
       <c r="G98" s="8"/>
-    </row>
-    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J98" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3908,8 +3987,11 @@
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="8"/>
-    </row>
-    <row r="100" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J99" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3927,8 +4009,11 @@
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="8"/>
-    </row>
-    <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J100" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3945,9 +4030,11 @@
         <v>3</v>
       </c>
       <c r="F101" s="2"/>
-      <c r="G101" s="8"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G101" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3965,8 +4052,11 @@
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="8"/>
-    </row>
-    <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J102" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3983,9 +4073,11 @@
         <v>3</v>
       </c>
       <c r="F103" s="2"/>
-      <c r="G103" s="8"/>
-    </row>
-    <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G103" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4003,8 +4095,11 @@
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="8"/>
-    </row>
-    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J104" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4022,8 +4117,11 @@
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="8"/>
-    </row>
-    <row r="106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J105" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4041,8 +4139,11 @@
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="8"/>
-    </row>
-    <row r="107" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J106" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4060,8 +4161,11 @@
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="8"/>
-    </row>
-    <row r="108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J107" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4079,8 +4183,11 @@
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="8"/>
-    </row>
-    <row r="109" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J108" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4100,8 +4207,11 @@
         <v>1</v>
       </c>
       <c r="G109" s="8"/>
-    </row>
-    <row r="110" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J109" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4119,8 +4229,11 @@
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="8"/>
-    </row>
-    <row r="111" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J110" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4138,8 +4251,11 @@
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="8"/>
-    </row>
-    <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J111" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4157,8 +4273,11 @@
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="8"/>
-    </row>
-    <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J112" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4176,8 +4295,11 @@
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="8"/>
-    </row>
-    <row r="114" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J113" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4195,8 +4317,11 @@
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="8"/>
-    </row>
-    <row r="115" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J114" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4216,8 +4341,11 @@
         <v>1</v>
       </c>
       <c r="G115" s="8"/>
-    </row>
-    <row r="116" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J115" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4237,8 +4365,11 @@
         <v>1</v>
       </c>
       <c r="G116" s="8"/>
-    </row>
-    <row r="117" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J116" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4256,8 +4387,11 @@
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="8"/>
-    </row>
-    <row r="118" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J117" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4275,8 +4409,11 @@
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="8"/>
-    </row>
-    <row r="119" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J118" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4294,8 +4431,11 @@
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="8"/>
-    </row>
-    <row r="120" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J119" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4313,8 +4453,11 @@
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="8"/>
-    </row>
-    <row r="121" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J120" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4332,8 +4475,11 @@
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="8"/>
-    </row>
-    <row r="122" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J121" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4353,8 +4499,11 @@
         <v>1</v>
       </c>
       <c r="G122" s="8"/>
-    </row>
-    <row r="123" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J122" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4372,8 +4521,11 @@
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="8"/>
-    </row>
-    <row r="124" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J123" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4391,8 +4543,11 @@
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="8"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J124" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4410,8 +4565,11 @@
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="8"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J125" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4431,8 +4589,11 @@
         <v>1</v>
       </c>
       <c r="G126" s="8"/>
-    </row>
-    <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J126" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4452,8 +4613,11 @@
         <v>1</v>
       </c>
       <c r="G127" s="8"/>
-    </row>
-    <row r="128" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J127" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4471,8 +4635,11 @@
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="8"/>
-    </row>
-    <row r="129" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J128" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4490,8 +4657,11 @@
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="8"/>
-    </row>
-    <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J129" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4509,8 +4679,11 @@
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="8"/>
-    </row>
-    <row r="131" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J130" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4528,8 +4701,11 @@
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="8"/>
-    </row>
-    <row r="132" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J131" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4549,8 +4725,11 @@
         <v>1</v>
       </c>
       <c r="G132" s="8"/>
-    </row>
-    <row r="133" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J132" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4568,8 +4747,11 @@
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="8"/>
-    </row>
-    <row r="134" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J133" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4587,8 +4769,11 @@
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="8"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J134" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4606,8 +4791,11 @@
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="8"/>
-    </row>
-    <row r="136" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J135" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4627,8 +4815,11 @@
         <v>1</v>
       </c>
       <c r="G136" s="8"/>
-    </row>
-    <row r="137" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J136" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4646,8 +4837,11 @@
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="8"/>
-    </row>
-    <row r="138" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J137" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4665,8 +4859,11 @@
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="8"/>
-    </row>
-    <row r="139" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J138" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4684,8 +4881,11 @@
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="8"/>
-    </row>
-    <row r="140" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J139" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4705,8 +4905,11 @@
         <v>1</v>
       </c>
       <c r="G140" s="8"/>
-    </row>
-    <row r="141" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J140" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4724,8 +4927,11 @@
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="8"/>
-    </row>
-    <row r="142" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J141" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4743,8 +4949,11 @@
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="8"/>
-    </row>
-    <row r="143" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J142" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4762,8 +4971,11 @@
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="8"/>
-    </row>
-    <row r="144" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J143" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4781,8 +4993,11 @@
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="8"/>
-    </row>
-    <row r="145" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J144" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4802,8 +5017,11 @@
         <v>1</v>
       </c>
       <c r="G145" s="8"/>
-    </row>
-    <row r="146" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J145" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4823,8 +5041,11 @@
         <v>1</v>
       </c>
       <c r="G146" s="8"/>
-    </row>
-    <row r="147" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J146" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4842,8 +5063,11 @@
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="8"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J147" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4861,8 +5085,11 @@
       </c>
       <c r="F148" s="2"/>
       <c r="G148" s="8"/>
-    </row>
-    <row r="149" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J148" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4880,8 +5107,11 @@
       </c>
       <c r="F149" s="2"/>
       <c r="G149" s="8"/>
-    </row>
-    <row r="150" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J149" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4899,8 +5129,11 @@
       </c>
       <c r="F150" s="2"/>
       <c r="G150" s="8"/>
-    </row>
-    <row r="151" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J150" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4918,8 +5151,11 @@
       </c>
       <c r="F151" s="2"/>
       <c r="G151" s="8"/>
-    </row>
-    <row r="152" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J151" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4937,8 +5173,11 @@
       </c>
       <c r="F152" s="2"/>
       <c r="G152" s="8"/>
-    </row>
-    <row r="153" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J152" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4958,8 +5197,11 @@
         <v>1</v>
       </c>
       <c r="G153" s="8"/>
-    </row>
-    <row r="154" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J153" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4977,8 +5219,11 @@
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="8"/>
-    </row>
-    <row r="155" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J154" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4998,8 +5243,11 @@
         <v>1</v>
       </c>
       <c r="G155" s="8"/>
-    </row>
-    <row r="156" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J155" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5017,8 +5265,11 @@
       </c>
       <c r="F156" s="2"/>
       <c r="G156" s="8"/>
-    </row>
-    <row r="157" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J156" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5036,8 +5287,11 @@
       </c>
       <c r="F157" s="2"/>
       <c r="G157" s="8"/>
-    </row>
-    <row r="158" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J157" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5055,8 +5309,11 @@
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="8"/>
-    </row>
-    <row r="159" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J158" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5074,8 +5331,11 @@
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="8"/>
-    </row>
-    <row r="160" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J159" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5093,8 +5353,11 @@
       </c>
       <c r="F160" s="2"/>
       <c r="G160" s="8"/>
-    </row>
-    <row r="161" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J160" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5114,8 +5377,11 @@
         <v>1</v>
       </c>
       <c r="G161" s="8"/>
-    </row>
-    <row r="162" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J161" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5135,8 +5401,11 @@
         <v>1</v>
       </c>
       <c r="G162" s="8"/>
-    </row>
-    <row r="163" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J162" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5154,8 +5423,11 @@
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="8"/>
-    </row>
-    <row r="164" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J163" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5173,8 +5445,11 @@
       </c>
       <c r="F164" s="2"/>
       <c r="G164" s="8"/>
-    </row>
-    <row r="165" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J164" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5192,8 +5467,11 @@
       </c>
       <c r="F165" s="2"/>
       <c r="G165" s="8"/>
-    </row>
-    <row r="166" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J165" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5211,8 +5489,11 @@
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="8"/>
-    </row>
-    <row r="167" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J166" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5232,8 +5513,11 @@
         <v>1</v>
       </c>
       <c r="G167" s="8"/>
-    </row>
-    <row r="168" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J167" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5253,8 +5537,11 @@
         <v>1</v>
       </c>
       <c r="G168" s="8"/>
-    </row>
-    <row r="169" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J168" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5274,8 +5561,11 @@
         <v>1</v>
       </c>
       <c r="G169" s="8"/>
-    </row>
-    <row r="170" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J169" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5293,8 +5583,11 @@
       </c>
       <c r="F170" s="2"/>
       <c r="G170" s="8"/>
-    </row>
-    <row r="171" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J170" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5312,8 +5605,11 @@
       </c>
       <c r="F171" s="2"/>
       <c r="G171" s="8"/>
-    </row>
-    <row r="172" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J171" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5331,8 +5627,11 @@
       </c>
       <c r="F172" s="2"/>
       <c r="G172" s="8"/>
-    </row>
-    <row r="173" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J172" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5350,8 +5649,11 @@
       </c>
       <c r="F173" s="2"/>
       <c r="G173" s="8"/>
-    </row>
-    <row r="174" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J173" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5369,8 +5671,11 @@
       </c>
       <c r="F174" s="2"/>
       <c r="G174" s="8"/>
-    </row>
-    <row r="175" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J174" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5388,8 +5693,11 @@
       </c>
       <c r="F175" s="2"/>
       <c r="G175" s="8"/>
-    </row>
-    <row r="176" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J175" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5407,8 +5715,11 @@
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="8"/>
-    </row>
-    <row r="177" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J176" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5428,8 +5739,11 @@
         <v>1</v>
       </c>
       <c r="G177" s="8"/>
-    </row>
-    <row r="178" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J177" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5449,8 +5763,11 @@
         <v>1</v>
       </c>
       <c r="G178" s="8"/>
-    </row>
-    <row r="179" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J178" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5468,8 +5785,11 @@
       </c>
       <c r="F179" s="2"/>
       <c r="G179" s="8"/>
-    </row>
-    <row r="180" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J179" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5487,8 +5807,11 @@
       </c>
       <c r="F180" s="2"/>
       <c r="G180" s="8"/>
-    </row>
-    <row r="181" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J180" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5506,8 +5829,11 @@
       </c>
       <c r="F181" s="2"/>
       <c r="G181" s="8"/>
-    </row>
-    <row r="182" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="J181" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5525,8 +5851,11 @@
       </c>
       <c r="F182" s="2"/>
       <c r="G182" s="8"/>
-    </row>
-    <row r="183" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="J182" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5545,7 +5874,7 @@
       </c>
       <c r="G183" s="8"/>
     </row>
-    <row r="184" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5566,7 +5895,7 @@
       </c>
       <c r="G184" s="8"/>
     </row>
-    <row r="185" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5587,7 +5916,7 @@
       </c>
       <c r="G185" s="8"/>
     </row>
-    <row r="186" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5608,7 +5937,7 @@
       </c>
       <c r="G186" s="8"/>
     </row>
-    <row r="187" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5627,7 +5956,7 @@
       <c r="F187" s="2"/>
       <c r="G187" s="8"/>
     </row>
-    <row r="188" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5646,7 +5975,7 @@
       <c r="F188" s="2"/>
       <c r="G188" s="8"/>
     </row>
-    <row r="189" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5665,7 +5994,7 @@
       <c r="F189" s="2"/>
       <c r="G189" s="8"/>
     </row>
-    <row r="190" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5684,7 +6013,7 @@
       <c r="F190" s="2"/>
       <c r="G190" s="8"/>
     </row>
-    <row r="191" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5703,7 +6032,7 @@
       <c r="F191" s="2"/>
       <c r="G191" s="8"/>
     </row>
-    <row r="192" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6742,7 +7071,7 @@
       <c r="A245">
         <v>244</v>
       </c>
-      <c r="B245" s="11" t="s">
+      <c r="B245" s="10" t="s">
         <v>321</v>
       </c>
       <c r="C245" s="4" t="s">

</xml_diff>